<commit_message>
MV MS to dp & dr profiles 9c88c3b9eefd988b262ec41f4352dc6c41dd4a59
</commit_message>
<xml_diff>
--- a/nr-mv-MS/ig/StructureDefinition-as-device.xlsx
+++ b/nr-mv-MS/ig/StructureDefinition-as-device.xlsx
@@ -9,9 +9,6 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$114</definedName>
-  </definedNames>
 </workbook>
 </file>
 
@@ -60,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-08T14:08:34+00:00</t>
+    <t>2025-10-08T14:26:13+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1905,21 +1902,6 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color indexed="22"/>
-        <i val="true"/>
-      </font>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -2268,7 +2250,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" hidden="true">
+    <row r="2">
       <c r="A2" t="s" s="2">
         <v>30</v>
       </c>
@@ -2380,7 +2362,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" hidden="true">
+    <row r="3">
       <c r="A3" t="s" s="2">
         <v>85</v>
       </c>
@@ -2494,7 +2476,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" hidden="true">
+    <row r="4">
       <c r="A4" t="s" s="2">
         <v>93</v>
       </c>
@@ -2606,7 +2588,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" hidden="true">
+    <row r="5">
       <c r="A5" t="s" s="2">
         <v>99</v>
       </c>
@@ -2718,7 +2700,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" hidden="true">
+    <row r="6">
       <c r="A6" t="s" s="2">
         <v>105</v>
       </c>
@@ -2853,7 +2835,7 @@
         <v>86</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I7" t="s" s="2">
         <v>77</v>
@@ -2946,7 +2928,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" hidden="true">
+    <row r="8">
       <c r="A8" t="s" s="2">
         <v>121</v>
       </c>
@@ -3060,7 +3042,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" hidden="true">
+    <row r="9">
       <c r="A9" t="s" s="2">
         <v>126</v>
       </c>
@@ -3174,7 +3156,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" hidden="true">
+    <row r="10">
       <c r="A10" t="s" s="2">
         <v>132</v>
       </c>
@@ -3288,7 +3270,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
         <v>138</v>
       </c>
@@ -3402,7 +3384,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" hidden="true">
+    <row r="12">
       <c r="A12" t="s" s="2">
         <v>144</v>
       </c>
@@ -3516,7 +3498,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
         <v>153</v>
       </c>
@@ -3630,7 +3612,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" hidden="true">
+    <row r="14">
       <c r="A14" t="s" s="2">
         <v>161</v>
       </c>
@@ -3744,7 +3726,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" hidden="true">
+    <row r="15">
       <c r="A15" t="s" s="2">
         <v>166</v>
       </c>
@@ -3858,7 +3840,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
         <v>175</v>
       </c>
@@ -3972,7 +3954,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>183</v>
       </c>
@@ -4086,7 +4068,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" hidden="true">
+    <row r="18">
       <c r="A18" t="s" s="2">
         <v>191</v>
       </c>
@@ -4217,7 +4199,7 @@
         <v>86</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>77</v>
@@ -4310,7 +4292,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" hidden="true">
+    <row r="20">
       <c r="A20" t="s" s="2">
         <v>201</v>
       </c>
@@ -4422,7 +4404,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" hidden="true">
+    <row r="21">
       <c r="A21" t="s" s="2">
         <v>203</v>
       </c>
@@ -4536,7 +4518,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
         <v>205</v>
       </c>
@@ -4650,7 +4632,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
         <v>208</v>
       </c>
@@ -4762,7 +4744,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" hidden="true">
+    <row r="24">
       <c r="A24" t="s" s="2">
         <v>210</v>
       </c>
@@ -4874,7 +4856,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" hidden="true">
+    <row r="25">
       <c r="A25" t="s" s="2">
         <v>212</v>
       </c>
@@ -4988,7 +4970,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" hidden="true">
+    <row r="26">
       <c r="A26" t="s" s="2">
         <v>218</v>
       </c>
@@ -5100,7 +5082,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" hidden="true">
+    <row r="27">
       <c r="A27" t="s" s="2">
         <v>224</v>
       </c>
@@ -5214,7 +5196,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" hidden="true">
+    <row r="28">
       <c r="A28" t="s" s="2">
         <v>226</v>
       </c>
@@ -5326,7 +5308,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" hidden="true">
+    <row r="29">
       <c r="A29" t="s" s="2">
         <v>227</v>
       </c>
@@ -5438,7 +5420,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" hidden="true">
+    <row r="30">
       <c r="A30" t="s" s="2">
         <v>228</v>
       </c>
@@ -5552,7 +5534,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" hidden="true">
+    <row r="31">
       <c r="A31" t="s" s="2">
         <v>229</v>
       </c>
@@ -5664,7 +5646,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" hidden="true">
+    <row r="32">
       <c r="A32" t="s" s="2">
         <v>231</v>
       </c>
@@ -5776,7 +5758,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" hidden="true">
+    <row r="33">
       <c r="A33" t="s" s="2">
         <v>233</v>
       </c>
@@ -5890,7 +5872,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" hidden="true">
+    <row r="34">
       <c r="A34" t="s" s="2">
         <v>235</v>
       </c>
@@ -6004,7 +5986,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" hidden="true">
+    <row r="35">
       <c r="A35" t="s" s="2">
         <v>245</v>
       </c>
@@ -6120,7 +6102,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" hidden="true">
+    <row r="36">
       <c r="A36" t="s" s="2">
         <v>254</v>
       </c>
@@ -6234,7 +6216,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" hidden="true">
+    <row r="37">
       <c r="A37" t="s" s="2">
         <v>257</v>
       </c>
@@ -6346,7 +6328,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" hidden="true">
+    <row r="38">
       <c r="A38" t="s" s="2">
         <v>258</v>
       </c>
@@ -6458,7 +6440,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" hidden="true">
+    <row r="39">
       <c r="A39" t="s" s="2">
         <v>259</v>
       </c>
@@ -6572,7 +6554,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" hidden="true">
+    <row r="40">
       <c r="A40" t="s" s="2">
         <v>260</v>
       </c>
@@ -6684,7 +6666,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" hidden="true">
+    <row r="41">
       <c r="A41" t="s" s="2">
         <v>261</v>
       </c>
@@ -6798,7 +6780,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" hidden="true">
+    <row r="42">
       <c r="A42" t="s" s="2">
         <v>264</v>
       </c>
@@ -6910,7 +6892,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" hidden="true">
+    <row r="43">
       <c r="A43" t="s" s="2">
         <v>265</v>
       </c>
@@ -7022,7 +7004,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" hidden="true">
+    <row r="44">
       <c r="A44" t="s" s="2">
         <v>266</v>
       </c>
@@ -7136,7 +7118,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" hidden="true">
+    <row r="45">
       <c r="A45" t="s" s="2">
         <v>267</v>
       </c>
@@ -7248,7 +7230,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" hidden="true">
+    <row r="46">
       <c r="A46" t="s" s="2">
         <v>269</v>
       </c>
@@ -7362,7 +7344,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" hidden="true">
+    <row r="47">
       <c r="A47" t="s" s="2">
         <v>272</v>
       </c>
@@ -7474,7 +7456,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" hidden="true">
+    <row r="48">
       <c r="A48" t="s" s="2">
         <v>275</v>
       </c>
@@ -7590,7 +7572,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" hidden="true">
+    <row r="49">
       <c r="A49" t="s" s="2">
         <v>280</v>
       </c>
@@ -7609,7 +7591,7 @@
         <v>79</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>77</v>
@@ -7704,7 +7686,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="50" hidden="true">
+    <row r="50">
       <c r="A50" t="s" s="2">
         <v>290</v>
       </c>
@@ -7820,7 +7802,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="51" hidden="true">
+    <row r="51">
       <c r="A51" t="s" s="2">
         <v>293</v>
       </c>
@@ -7932,7 +7914,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" hidden="true">
+    <row r="52">
       <c r="A52" t="s" s="2">
         <v>295</v>
       </c>
@@ -8046,7 +8028,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" hidden="true">
+    <row r="53">
       <c r="A53" t="s" s="2">
         <v>297</v>
       </c>
@@ -8162,7 +8144,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" hidden="true">
+    <row r="54">
       <c r="A54" t="s" s="2">
         <v>308</v>
       </c>
@@ -8278,7 +8260,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" hidden="true">
+    <row r="55">
       <c r="A55" t="s" s="2">
         <v>318</v>
       </c>
@@ -8394,7 +8376,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" hidden="true">
+    <row r="56">
       <c r="A56" t="s" s="2">
         <v>328</v>
       </c>
@@ -8508,7 +8490,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="57" hidden="true">
+    <row r="57">
       <c r="A57" t="s" s="2">
         <v>337</v>
       </c>
@@ -8620,7 +8602,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" hidden="true">
+    <row r="58">
       <c r="A58" t="s" s="2">
         <v>343</v>
       </c>
@@ -8734,7 +8716,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" hidden="true">
+    <row r="59">
       <c r="A59" t="s" s="2">
         <v>351</v>
       </c>
@@ -8846,7 +8828,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" hidden="true">
+    <row r="60">
       <c r="A60" t="s" s="2">
         <v>355</v>
       </c>
@@ -8960,7 +8942,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" hidden="true">
+    <row r="61">
       <c r="A61" t="s" s="2">
         <v>361</v>
       </c>
@@ -9072,7 +9054,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="62" hidden="true">
+    <row r="62">
       <c r="A62" t="s" s="2">
         <v>362</v>
       </c>
@@ -9186,7 +9168,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" hidden="true">
+    <row r="63">
       <c r="A63" t="s" s="2">
         <v>363</v>
       </c>
@@ -9302,7 +9284,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="64" hidden="true">
+    <row r="64">
       <c r="A64" t="s" s="2">
         <v>368</v>
       </c>
@@ -9414,7 +9396,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="65" hidden="true">
+    <row r="65">
       <c r="A65" t="s" s="2">
         <v>375</v>
       </c>
@@ -9526,7 +9508,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="66" hidden="true">
+    <row r="66">
       <c r="A66" t="s" s="2">
         <v>381</v>
       </c>
@@ -9640,7 +9622,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" hidden="true">
+    <row r="67">
       <c r="A67" t="s" s="2">
         <v>386</v>
       </c>
@@ -9754,7 +9736,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="68" hidden="true">
+    <row r="68">
       <c r="A68" t="s" s="2">
         <v>393</v>
       </c>
@@ -9868,7 +9850,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="69" hidden="true">
+    <row r="69">
       <c r="A69" t="s" s="2">
         <v>399</v>
       </c>
@@ -10001,7 +9983,7 @@
         <v>86</v>
       </c>
       <c r="H70" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I70" t="s" s="2">
         <v>87</v>
@@ -10096,7 +10078,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" hidden="true">
+    <row r="71">
       <c r="A71" t="s" s="2">
         <v>414</v>
       </c>
@@ -10208,7 +10190,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="72" hidden="true">
+    <row r="72">
       <c r="A72" t="s" s="2">
         <v>419</v>
       </c>
@@ -10341,7 +10323,7 @@
         <v>86</v>
       </c>
       <c r="H73" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I73" t="s" s="2">
         <v>77</v>
@@ -10434,7 +10416,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="74" hidden="true">
+    <row r="74">
       <c r="A74" t="s" s="2">
         <v>431</v>
       </c>
@@ -10546,7 +10528,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="75" hidden="true">
+    <row r="75">
       <c r="A75" t="s" s="2">
         <v>436</v>
       </c>
@@ -10658,7 +10640,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="76" hidden="true">
+    <row r="76">
       <c r="A76" t="s" s="2">
         <v>441</v>
       </c>
@@ -10789,7 +10771,7 @@
         <v>86</v>
       </c>
       <c r="H77" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I77" t="s" s="2">
         <v>77</v>
@@ -10884,7 +10866,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" hidden="true">
+    <row r="78">
       <c r="A78" t="s" s="2">
         <v>450</v>
       </c>
@@ -10996,7 +10978,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" hidden="true">
+    <row r="79">
       <c r="A79" t="s" s="2">
         <v>453</v>
       </c>
@@ -11108,7 +11090,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" hidden="true">
+    <row r="80">
       <c r="A80" t="s" s="2">
         <v>454</v>
       </c>
@@ -11222,7 +11204,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="81" hidden="true">
+    <row r="81">
       <c r="A81" t="s" s="2">
         <v>455</v>
       </c>
@@ -11338,7 +11320,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="82" hidden="true">
+    <row r="82">
       <c r="A82" t="s" s="2">
         <v>456</v>
       </c>
@@ -11450,7 +11432,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="83" hidden="true">
+    <row r="83">
       <c r="A83" t="s" s="2">
         <v>460</v>
       </c>
@@ -11562,7 +11544,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="84" hidden="true">
+    <row r="84">
       <c r="A84" t="s" s="2">
         <v>466</v>
       </c>
@@ -11674,7 +11656,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" hidden="true">
+    <row r="85">
       <c r="A85" t="s" s="2">
         <v>470</v>
       </c>
@@ -11807,7 +11789,7 @@
         <v>86</v>
       </c>
       <c r="H86" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I86" t="s" s="2">
         <v>77</v>
@@ -11898,7 +11880,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="87" hidden="true">
+    <row r="87">
       <c r="A87" t="s" s="2">
         <v>478</v>
       </c>
@@ -12010,7 +11992,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="88" hidden="true">
+    <row r="88">
       <c r="A88" t="s" s="2">
         <v>481</v>
       </c>
@@ -12122,7 +12104,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="89" hidden="true">
+    <row r="89">
       <c r="A89" t="s" s="2">
         <v>482</v>
       </c>
@@ -12236,7 +12218,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="90" hidden="true">
+    <row r="90">
       <c r="A90" t="s" s="2">
         <v>483</v>
       </c>
@@ -12352,7 +12334,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" hidden="true">
+    <row r="91">
       <c r="A91" t="s" s="2">
         <v>484</v>
       </c>
@@ -12464,7 +12446,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="92" hidden="true">
+    <row r="92">
       <c r="A92" t="s" s="2">
         <v>487</v>
       </c>
@@ -12576,7 +12558,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="93" hidden="true">
+    <row r="93">
       <c r="A93" t="s" s="2">
         <v>490</v>
       </c>
@@ -12688,7 +12670,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="94" hidden="true">
+    <row r="94">
       <c r="A94" t="s" s="2">
         <v>493</v>
       </c>
@@ -12800,7 +12782,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="95" hidden="true">
+    <row r="95">
       <c r="A95" t="s" s="2">
         <v>494</v>
       </c>
@@ -12914,7 +12896,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="96" hidden="true">
+    <row r="96">
       <c r="A96" t="s" s="2">
         <v>495</v>
       </c>
@@ -13030,7 +13012,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="97" hidden="true">
+    <row r="97">
       <c r="A97" t="s" s="2">
         <v>496</v>
       </c>
@@ -13142,7 +13124,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="98" hidden="true">
+    <row r="98">
       <c r="A98" t="s" s="2">
         <v>499</v>
       </c>
@@ -13254,7 +13236,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="99" hidden="true">
+    <row r="99">
       <c r="A99" t="s" s="2">
         <v>502</v>
       </c>
@@ -13366,7 +13348,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="100" hidden="true">
+    <row r="100">
       <c r="A100" t="s" s="2">
         <v>505</v>
       </c>
@@ -13478,7 +13460,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="101" hidden="true">
+    <row r="101">
       <c r="A101" t="s" s="2">
         <v>508</v>
       </c>
@@ -13590,7 +13572,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="102" hidden="true">
+    <row r="102">
       <c r="A102" t="s" s="2">
         <v>509</v>
       </c>
@@ -13704,7 +13686,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="103" hidden="true">
+    <row r="103">
       <c r="A103" t="s" s="2">
         <v>510</v>
       </c>
@@ -13820,7 +13802,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="104" hidden="true">
+    <row r="104">
       <c r="A104" t="s" s="2">
         <v>511</v>
       </c>
@@ -13932,7 +13914,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="105" hidden="true">
+    <row r="105">
       <c r="A105" t="s" s="2">
         <v>514</v>
       </c>
@@ -14044,7 +14026,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="106" hidden="true">
+    <row r="106">
       <c r="A106" t="s" s="2">
         <v>518</v>
       </c>
@@ -14156,7 +14138,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="107" hidden="true">
+    <row r="107">
       <c r="A107" t="s" s="2">
         <v>521</v>
       </c>
@@ -14289,7 +14271,7 @@
         <v>86</v>
       </c>
       <c r="H108" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I108" t="s" s="2">
         <v>77</v>
@@ -14382,7 +14364,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="109" hidden="true">
+    <row r="109">
       <c r="A109" t="s" s="2">
         <v>534</v>
       </c>
@@ -14496,7 +14478,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="110" hidden="true">
+    <row r="110">
       <c r="A110" t="s" s="2">
         <v>540</v>
       </c>
@@ -14610,7 +14592,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="111" hidden="true">
+    <row r="111">
       <c r="A111" t="s" s="2">
         <v>547</v>
       </c>
@@ -14724,7 +14706,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="112" hidden="true">
+    <row r="112">
       <c r="A112" t="s" s="2">
         <v>552</v>
       </c>
@@ -14836,7 +14818,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" hidden="true">
+    <row r="113">
       <c r="A113" t="s" s="2">
         <v>557</v>
       </c>
@@ -14948,7 +14930,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="114" hidden="true">
+    <row r="114">
       <c r="A114" t="s" s="2">
         <v>560</v>
       </c>
@@ -15061,24 +15043,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN114">
-    <filterColumn colId="7">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="27">
-      <filters blank="true"/>
-    </filterColumn>
-  </autoFilter>
-  <conditionalFormatting sqref="A2:AI113">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$G2&lt;&gt;"Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$Q2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>